<commit_message>
Update AnalisiReq, Glossario e Tempi di Lavoro
</commit_message>
<xml_diff>
--- a/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_LucaB.xlsx
+++ b/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_LucaB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Documenti\GitHub\GDPRProject\Documentazione\GDPRPrj_TempiLavoro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E89A74-9701-4D16-97E0-E456C9782E2D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08286B5E-26DE-4D47-9D80-FC4F5796023C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="10">
   <si>
     <t>Persona</t>
   </si>
@@ -416,7 +416,7 @@
   <dimension ref="E1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -647,7 +647,21 @@
       </c>
     </row>
     <row r="14" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="H14" s="1"/>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="1">
+        <v>43553</v>
+      </c>
+      <c r="I14">
+        <v>60</v>
+      </c>
     </row>
     <row r="15" spans="5:9" x14ac:dyDescent="0.3">
       <c r="H15" s="1"/>

</xml_diff>